<commit_message>
Remove population and add it to lookup-tables
</commit_message>
<xml_diff>
--- a/data/00_lookup_tables_and_maps/01_lookup_tables/msis.xlsx
+++ b/data/00_lookup_tables_and_maps/01_lookup_tables/msis.xlsx
@@ -400,7 +400,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>geometry</t>
+          <t>population</t>
         </is>
       </c>
     </row>
@@ -445,6 +445,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I2">
+        <v>58671</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -487,6 +490,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I3">
+        <v>62423</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -529,6 +535,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I4">
+        <v>45089</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -571,6 +580,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I5">
+        <v>38945</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -613,6 +625,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I6">
+        <v>59269</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -655,6 +670,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I7">
+        <v>34569</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -697,6 +715,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I8">
+        <v>50157</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -739,6 +760,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I9">
+        <v>52327</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -781,6 +805,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I10">
+        <v>33422</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -823,6 +850,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I11">
+        <v>27707</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -865,6 +895,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I12">
+        <v>33316</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -907,6 +940,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I13">
+        <v>49801</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -949,6 +985,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I14">
+        <v>50806</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -991,6 +1030,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I15">
+        <v>52459</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1033,6 +1075,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I16">
+        <v>39066</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1075,6 +1120,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I17">
+        <v>1471</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1117,6 +1165,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I18">
+        <v>1610</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1159,6 +1210,9 @@
           <t>Oslo</t>
         </is>
       </c>
+      <c r="I19">
+        <v>2386</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1191,6 +1245,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I20">
+        <v>14811</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1223,6 +1280,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I21">
+        <v>143574</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1255,6 +1315,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I22">
+        <v>37357</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1287,6 +1350,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I23">
+        <v>79537</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1319,6 +1385,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I24">
+        <v>3280</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1351,6 +1420,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I25">
+        <v>3202</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1383,6 +1455,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I26">
+        <v>2787</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1415,6 +1490,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I27">
+        <v>18991</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1447,6 +1525,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I28">
+        <v>19588</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1479,6 +1560,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I29">
+        <v>18916</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1511,6 +1595,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I30">
+        <v>12002</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1543,6 +1630,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I31">
+        <v>27153</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1575,6 +1665,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I32">
+        <v>11221</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1607,6 +1700,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I33">
+        <v>12968</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1639,6 +1735,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I34">
+        <v>2574</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1671,6 +1770,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I35">
+        <v>3804</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1703,6 +1805,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I36">
+        <v>4595</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1735,6 +1840,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I37">
+        <v>517</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1767,6 +1875,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I38">
+        <v>852</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1799,6 +1910,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I39">
+        <v>11065</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1831,6 +1945,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I40">
+        <v>42186</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1863,6 +1980,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I41">
+        <v>198</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1895,6 +2015,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="I42">
+        <v>8714</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1927,6 +2050,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I43">
+        <v>24179</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1959,6 +2085,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I44">
+        <v>31967</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1991,6 +2120,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I45">
+        <v>66258</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2023,6 +2155,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I46">
+        <v>3117</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2055,6 +2190,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I47">
+        <v>2461</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2087,6 +2225,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I48">
+        <v>8900</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2119,6 +2260,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I49">
+        <v>8571</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2151,6 +2295,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I50">
+        <v>5175</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2183,6 +2330,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I51">
+        <v>10825</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2215,6 +2365,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I52">
+        <v>4523</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2247,6 +2400,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I53">
+        <v>7625</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2279,6 +2435,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I54">
+        <v>9310</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2311,6 +2470,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I55">
+        <v>8462</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2343,6 +2505,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I56">
+        <v>6532</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2375,6 +2540,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I57">
+        <v>7468</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2407,6 +2575,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I58">
+        <v>3509</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2439,6 +2610,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I59">
+        <v>5788</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2471,6 +2645,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I60">
+        <v>2629</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2503,6 +2680,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I61">
+        <v>3025</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2535,6 +2715,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I62">
+        <v>7036</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2567,6 +2750,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I63">
+        <v>5920</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2599,6 +2785,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I64">
+        <v>2150</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2631,6 +2820,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I65">
+        <v>3507</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2663,6 +2855,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I66">
+        <v>10473</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2695,6 +2890,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I67">
+        <v>2549</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2727,6 +2925,9 @@
           <t>Møre og Romsdal</t>
         </is>
       </c>
+      <c r="I68">
+        <v>13279</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2759,6 +2960,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I69">
+        <v>52357</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2791,6 +2995,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I70">
+        <v>21845</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2823,6 +3030,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I71">
+        <v>1426</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2855,6 +3065,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I72">
+        <v>1975</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2887,6 +3100,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I73">
+        <v>7917</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2919,6 +3135,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I74">
+        <v>1200</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2951,6 +3170,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I75">
+        <v>462</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2983,6 +3205,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I76">
+        <v>1777</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3015,6 +3240,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I77">
+        <v>7447</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3047,6 +3275,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I78">
+        <v>2294</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3079,6 +3310,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I79">
+        <v>13278</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3111,6 +3345,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I80">
+        <v>1482</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3143,6 +3380,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I81">
+        <v>1297</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3175,6 +3415,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I82">
+        <v>1371</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3207,6 +3450,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I83">
+        <v>1761</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3239,6 +3485,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I84">
+        <v>4454</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3271,6 +3520,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I85">
+        <v>26184</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3303,6 +3555,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I86">
+        <v>1890</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3335,6 +3590,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I87">
+        <v>435</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3367,6 +3625,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I88">
+        <v>1213</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3399,6 +3660,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I89">
+        <v>6288</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3431,6 +3695,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I90">
+        <v>1950</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3463,6 +3730,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I91">
+        <v>1017</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3495,6 +3765,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I92">
+        <v>4671</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3527,6 +3800,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I93">
+        <v>9739</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3559,6 +3835,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I94">
+        <v>1926</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3591,6 +3870,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I95">
+        <v>2608</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3623,6 +3905,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I96">
+        <v>2034</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3655,6 +3940,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I97">
+        <v>1348</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3687,6 +3975,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I98">
+        <v>498</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3719,6 +4010,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I99">
+        <v>728</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3751,6 +4045,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I100">
+        <v>1272</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3783,6 +4080,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I101">
+        <v>11433</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3815,6 +4115,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I102">
+        <v>9608</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3847,6 +4150,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I103">
+        <v>8061</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3879,6 +4185,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I104">
+        <v>2569</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3911,6 +4220,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I105">
+        <v>4410</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3943,6 +4255,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I106">
+        <v>10566</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3975,6 +4290,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I107">
+        <v>4663</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4007,6 +4325,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I108">
+        <v>1015</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4039,6 +4360,9 @@
           <t>Nordland</t>
         </is>
       </c>
+      <c r="I109">
+        <v>2766</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4071,6 +4395,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I110">
+        <v>31373</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4103,6 +4430,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I111">
+        <v>49273</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4135,6 +4465,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I112">
+        <v>56732</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4167,6 +4500,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I113">
+        <v>82385</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -4199,6 +4535,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I114">
+        <v>101386</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -4231,6 +4570,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I115">
+        <v>27723</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -4263,6 +4605,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I116">
+        <v>30641</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -4295,6 +4640,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I117">
+        <v>4668</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -4327,6 +4675,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I118">
+        <v>1325</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -4359,6 +4710,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I119">
+        <v>3595</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -4391,6 +4745,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I120">
+        <v>44792</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -4423,6 +4780,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I121">
+        <v>3805</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -4455,6 +4815,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I122">
+        <v>8255</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -4487,6 +4850,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I123">
+        <v>7508</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -4519,6 +4885,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I124">
+        <v>5736</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -4551,6 +4920,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I125">
+        <v>18042</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -4583,6 +4955,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I126">
+        <v>59288</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -4615,6 +4990,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I127">
+        <v>20439</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -4647,6 +5025,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I128">
+        <v>15877</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -4679,6 +5060,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I129">
+        <v>19616</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -4711,6 +5095,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I130">
+        <v>127731</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -4743,6 +5130,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I131">
+        <v>94441</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -4775,6 +5165,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I132">
+        <v>17390</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -4807,6 +5200,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I133">
+        <v>18530</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -4839,6 +5235,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I134">
+        <v>11110</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -4871,6 +5270,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I135">
+        <v>41460</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -4903,6 +5305,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I136">
+        <v>85983</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -4935,6 +5340,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I137">
+        <v>24249</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -4967,6 +5375,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I138">
+        <v>6890</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -4999,6 +5410,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I139">
+        <v>39625</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -5031,6 +5445,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I140">
+        <v>23092</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -5063,6 +5480,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I141">
+        <v>25436</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -5095,6 +5515,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I142">
+        <v>14139</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -5127,6 +5550,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I143">
+        <v>2854</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -5159,6 +5585,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I144">
+        <v>6799</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -5191,6 +5620,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I145">
+        <v>1050</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -5223,6 +5655,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I146">
+        <v>3273</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -5255,6 +5690,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I147">
+        <v>4608</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -5287,6 +5725,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I148">
+        <v>2486</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -5319,6 +5760,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I149">
+        <v>4674</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -5351,6 +5795,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I150">
+        <v>4441</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -5383,6 +5830,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I151">
+        <v>3467</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -5415,6 +5865,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I152">
+        <v>2212</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -5447,6 +5900,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I153">
+        <v>14115</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -5479,6 +5935,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I154">
+        <v>19423</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -5511,6 +5970,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I155">
+        <v>26811</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -5543,6 +6005,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I156">
+        <v>2688</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -5575,6 +6040,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I157">
+        <v>1390</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -5607,6 +6075,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I158">
+        <v>2439</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -5639,6 +6110,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I159">
+        <v>6852</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -5671,6 +6145,9 @@
           <t>Viken</t>
         </is>
       </c>
+      <c r="I160">
+        <v>9048</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -5703,6 +6180,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I161">
+        <v>17829</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -5735,6 +6215,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I162">
+        <v>31369</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -5767,6 +6250,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I163">
+        <v>28345</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -5799,6 +6285,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I164">
+        <v>30560</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -5831,6 +6320,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I165">
+        <v>34768</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -5863,6 +6355,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I166">
+        <v>7674</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -5895,6 +6390,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I167">
+        <v>21064</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -5927,6 +6425,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I168">
+        <v>5016</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -5959,6 +6460,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I169">
+        <v>7905</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -5991,6 +6495,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I170">
+        <v>6106</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -6023,6 +6530,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I171">
+        <v>4612</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -6055,6 +6565,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I172">
+        <v>7203</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -6087,6 +6600,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I173">
+        <v>3662</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -6119,6 +6635,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I174">
+        <v>21254</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -6151,6 +6670,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I175">
+        <v>6627</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -6183,6 +6705,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I176">
+        <v>4356</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -6215,6 +6740,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I177">
+        <v>2419</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -6247,6 +6775,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I178">
+        <v>1780</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -6279,6 +6810,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I179">
+        <v>1268</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -6311,6 +6845,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I180">
+        <v>1562</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -6343,6 +6880,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I181">
+        <v>5578</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -6375,6 +6915,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I182">
+        <v>2432</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -6407,6 +6950,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I183">
+        <v>1545</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -6439,6 +6985,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I184">
+        <v>1891</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -6471,6 +7020,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I185">
+        <v>2553</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -6503,6 +7055,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I186">
+        <v>1975</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -6535,6 +7090,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I187">
+        <v>2197</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -6567,6 +7125,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I188">
+        <v>2228</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -6599,6 +7160,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I189">
+        <v>3570</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -6631,6 +7195,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I190">
+        <v>5723</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -6663,6 +7230,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I191">
+        <v>5739</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -6695,6 +7265,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I192">
+        <v>3119</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -6727,6 +7300,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I193">
+        <v>4392</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -6759,6 +7335,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I194">
+        <v>5100</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -6791,6 +7370,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I195">
+        <v>6106</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -6823,6 +7405,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I196">
+        <v>14973</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -6855,6 +7440,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I197">
+        <v>13427</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -6887,6 +7475,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I198">
+        <v>13630</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -6919,6 +7510,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I199">
+        <v>5617</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -6951,6 +7545,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I200">
+        <v>6633</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -6983,6 +7580,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I201">
+        <v>2954</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -7015,6 +7615,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I202">
+        <v>1279</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -7047,6 +7650,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I203">
+        <v>6413</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -7079,6 +7685,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I204">
+        <v>2125</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -7111,6 +7720,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I205">
+        <v>3229</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -7143,6 +7755,9 @@
           <t>Innlandet</t>
         </is>
       </c>
+      <c r="I206">
+        <v>1578</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -7175,6 +7790,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I207">
+        <v>27351</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -7207,6 +7825,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I208">
+        <v>24699</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -7239,6 +7860,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I209">
+        <v>56293</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -7271,6 +7895,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I210">
+        <v>63764</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -7303,6 +7930,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I211">
+        <v>47204</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -7335,6 +7965,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I212">
+        <v>36397</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -7367,6 +8000,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I213">
+        <v>54942</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -7399,6 +8035,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I214">
+        <v>13049</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -7431,6 +8070,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I215">
+        <v>26730</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -7463,6 +8105,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I216">
+        <v>2340</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -7495,6 +8140,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I217">
+        <v>14061</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -7527,6 +8175,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I218">
+        <v>10380</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -7559,6 +8210,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I219">
+        <v>4060</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -7591,6 +8245,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I220">
+        <v>6515</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -7623,6 +8280,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I221">
+        <v>10444</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -7655,6 +8315,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I222">
+        <v>5691</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -7687,6 +8350,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I223">
+        <v>1573</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -7719,6 +8385,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I224">
+        <v>2888</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -7751,6 +8420,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I225">
+        <v>2403</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -7783,6 +8455,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I226">
+        <v>1448</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -7815,6 +8490,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I227">
+        <v>1287</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -7847,6 +8525,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I228">
+        <v>2201</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -7879,6 +8560,9 @@
           <t>Vestfold og Telemark</t>
         </is>
       </c>
+      <c r="I229">
+        <v>3676</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -7911,6 +8595,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I230">
+        <v>6809</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -7943,6 +8630,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I231">
+        <v>23544</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -7975,6 +8665,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I232">
+        <v>44999</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -8007,6 +8700,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I233">
+        <v>111633</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -8039,6 +8735,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I234">
+        <v>23046</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -8071,6 +8770,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I235">
+        <v>9691</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -8103,6 +8805,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I236">
+        <v>9028</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -8135,6 +8840,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I237">
+        <v>2428</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -8167,6 +8875,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I238">
+        <v>2097</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -8199,6 +8910,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I239">
+        <v>6053</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -8231,6 +8945,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I240">
+        <v>5951</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -8263,6 +8980,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I241">
+        <v>11074</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -8295,6 +9015,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I242">
+        <v>5226</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -8327,6 +9050,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I243">
+        <v>1836</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -8359,6 +9085,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I244">
+        <v>1331</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -8391,6 +9120,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I245">
+        <v>3634</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -8423,6 +9155,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I246">
+        <v>1162</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -8455,6 +9190,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I247">
+        <v>1164</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -8487,6 +9225,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I248">
+        <v>965</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -8519,6 +9260,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I249">
+        <v>14774</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -8551,6 +9295,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I250">
+        <v>932</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -8583,6 +9330,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I251">
+        <v>10365</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -8615,6 +9365,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I252">
+        <v>1680</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -8647,6 +9400,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I253">
+        <v>5987</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -8679,6 +9435,9 @@
           <t>Agder</t>
         </is>
       </c>
+      <c r="I254">
+        <v>1822</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -8721,6 +9480,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I255">
+        <v>13820</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -8763,6 +9525,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I256">
+        <v>42790</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -8805,6 +9570,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I257">
+        <v>43139</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -8847,6 +9615,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I258">
+        <v>30071</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -8889,6 +9660,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I259">
+        <v>40409</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -8931,6 +9705,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I260">
+        <v>29279</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -8973,6 +9750,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I261">
+        <v>42223</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -9015,6 +9795,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I262">
+        <v>41629</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -9057,6 +9840,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I263">
+        <v>569</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -9089,6 +9875,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I264">
+        <v>17207</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -9121,6 +9910,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I265">
+        <v>4062</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -9153,6 +9945,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I266">
+        <v>5766</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -9185,6 +9980,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I267">
+        <v>11957</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -9217,6 +10015,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I268">
+        <v>18759</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -9249,6 +10050,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I269">
+        <v>3189</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -9281,6 +10085,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I270">
+        <v>2869</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -9313,6 +10120,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I271">
+        <v>13071</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -9345,6 +10155,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I272">
+        <v>11048</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -9377,6 +10190,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I273">
+        <v>906</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -9409,6 +10225,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I274">
+        <v>1080</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -9441,6 +10260,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I275">
+        <v>15740</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -9473,6 +10295,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I276">
+        <v>8457</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -9505,6 +10330,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I277">
+        <v>2485</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -9537,6 +10365,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I278">
+        <v>24908</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -9569,6 +10400,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I279">
+        <v>5236</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -9601,6 +10435,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I280">
+        <v>38316</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -9633,6 +10470,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I281">
+        <v>29553</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -9665,6 +10505,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I282">
+        <v>3977</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -9697,6 +10540,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I283">
+        <v>388</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -9729,6 +10575,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I284">
+        <v>8098</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -9761,6 +10610,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I285">
+        <v>29224</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -9793,6 +10645,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I286">
+        <v>2870</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -9825,6 +10680,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I287">
+        <v>548</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -9857,6 +10715,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I288">
+        <v>1691</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -9889,6 +10750,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I289">
+        <v>2297</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -9921,6 +10785,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I290">
+        <v>802</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -9953,6 +10820,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I291">
+        <v>1328</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -9985,6 +10855,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I292">
+        <v>4101</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -10017,6 +10890,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I293">
+        <v>2635</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -10049,6 +10925,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I294">
+        <v>11847</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -10081,6 +10960,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I295">
+        <v>1781</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -10113,6 +10995,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I296">
+        <v>2126</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -10145,6 +11030,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I297">
+        <v>5193</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -10177,6 +11065,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I298">
+        <v>5174</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -10209,6 +11100,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I299">
+        <v>3011</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -10241,6 +11135,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I300">
+        <v>2802</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -10273,6 +11170,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I301">
+        <v>22030</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -10305,6 +11205,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I302">
+        <v>3629</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -10337,6 +11240,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I303">
+        <v>9457</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -10369,6 +11275,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I304">
+        <v>5854</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -10401,6 +11310,9 @@
           <t>Vestland</t>
         </is>
       </c>
+      <c r="I305">
+        <v>7130</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -10433,6 +11345,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I306">
+        <v>205163</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -10465,6 +11380,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I307">
+        <v>24357</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -10497,6 +11415,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I308">
+        <v>15230</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -10529,6 +11450,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I309">
+        <v>5151</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -10561,6 +11485,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I310">
+        <v>948</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -10593,6 +11520,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I311">
+        <v>7001</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -10625,6 +11555,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I312">
+        <v>2486</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -10657,6 +11590,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I313">
+        <v>5581</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -10689,6 +11625,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I314">
+        <v>1981</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -10721,6 +11660,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I315">
+        <v>6238</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -10753,6 +11695,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I316">
+        <v>16733</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -10785,6 +11730,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I317">
+        <v>8325</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -10817,6 +11765,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I318">
+        <v>14148</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -10849,6 +11800,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I319">
+        <v>4062</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -10881,6 +11835,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I320">
+        <v>769</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -10913,6 +11870,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I321">
+        <v>2422</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -10945,6 +11905,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I322">
+        <v>24145</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -10977,6 +11940,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I323">
+        <v>2627</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -11009,6 +11975,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I324">
+        <v>20164</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -11041,6 +12010,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I325">
+        <v>14948</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -11073,6 +12045,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I326">
+        <v>2063</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -11105,6 +12080,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I327">
+        <v>1355</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -11137,6 +12115,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I328">
+        <v>461</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -11169,6 +12150,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I329">
+        <v>843</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -11201,6 +12185,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I330">
+        <v>2359</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -11233,6 +12220,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I331">
+        <v>1231</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -11265,6 +12255,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I332">
+        <v>3884</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -11297,6 +12290,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I333">
+        <v>1103</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -11329,6 +12325,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I334">
+        <v>557</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -11361,6 +12360,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I335">
+        <v>6816</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -11393,6 +12395,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I336">
+        <v>10084</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -11425,6 +12430,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I337">
+        <v>5963</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -11457,6 +12465,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I338">
+        <v>5050</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -11489,6 +12500,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I339">
+        <v>10323</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -11521,6 +12535,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I340">
+        <v>4288</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -11553,6 +12570,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I341">
+        <v>18217</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -11585,6 +12605,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I342">
+        <v>9623</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
@@ -11617,6 +12640,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="I343">
+        <v>2003</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -11649,6 +12675,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I344">
+        <v>76974</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -11681,6 +12710,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I345">
+        <v>24703</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -11713,6 +12745,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I346">
+        <v>20789</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -11745,6 +12780,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I347">
+        <v>2029</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -11777,6 +12815,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I348">
+        <v>5788</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
@@ -11809,6 +12850,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I349">
+        <v>11448</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -11841,6 +12885,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I350">
+        <v>2839</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -11873,6 +12920,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I351">
+        <v>4216</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
@@ -11905,6 +12955,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I352">
+        <v>1361</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
@@ -11937,6 +12990,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I353">
+        <v>1091</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -11969,6 +13025,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I354">
+        <v>1034</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -12001,6 +13060,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I355">
+        <v>4005</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -12033,6 +13095,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I356">
+        <v>2146</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -12065,6 +13130,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I357">
+        <v>6640</v>
+      </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -12097,6 +13165,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I358">
+        <v>3464</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -12129,6 +13200,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I359">
+        <v>1083</v>
+      </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
@@ -12161,6 +13235,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I360">
+        <v>14851</v>
+      </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
@@ -12193,6 +13270,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I361">
+        <v>5559</v>
+      </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
@@ -12225,6 +13305,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I362">
+        <v>2200</v>
+      </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -12257,6 +13340,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I363">
+        <v>2794</v>
+      </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
@@ -12289,6 +13375,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I364">
+        <v>1829</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -12321,6 +13410,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I365">
+        <v>2071</v>
+      </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
@@ -12353,6 +13445,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I366">
+        <v>2927</v>
+      </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
@@ -12385,6 +13480,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I367">
+        <v>4861</v>
+      </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
@@ -12417,6 +13515,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I368">
+        <v>1191</v>
+      </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -12449,6 +13550,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I369">
+        <v>2910</v>
+      </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -12481,6 +13585,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I370">
+        <v>888</v>
+      </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
@@ -12513,6 +13620,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I371">
+        <v>1005</v>
+      </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
@@ -12545,6 +13655,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I372">
+        <v>1225</v>
+      </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
@@ -12577,6 +13690,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I373">
+        <v>3162</v>
+      </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
@@ -12609,6 +13725,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I374">
+        <v>3998</v>
+      </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -12641,6 +13760,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I375">
+        <v>2628</v>
+      </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -12673,6 +13795,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I376">
+        <v>1290</v>
+      </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
@@ -12705,6 +13830,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I377">
+        <v>1132</v>
+      </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
@@ -12737,6 +13865,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I378">
+        <v>957</v>
+      </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
@@ -12769,6 +13900,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I379">
+        <v>2918</v>
+      </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
@@ -12801,6 +13935,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I380">
+        <v>926</v>
+      </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -12833,6 +13970,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I381">
+        <v>2221</v>
+      </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
@@ -12865,6 +14005,9 @@
           <t>Troms og Finnmark</t>
         </is>
       </c>
+      <c r="I382">
+        <v>10158</v>
+      </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
@@ -12897,6 +14040,9 @@
           <t>Svalbard</t>
         </is>
       </c>
+      <c r="I383">
+        <v>0</v>
+      </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
@@ -12928,6 +14074,9 @@
         <is>
           <t>Ukjent Fylke</t>
         </is>
+      </c>
+      <c r="I384">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>